<commit_message>
Add assembly and installation-related inputs.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-wind-turbines.xlsx
+++ b/premise/data/additional_inventories/lci-wind-turbines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise-johanna/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise-johanna/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7826F2B-281D-074B-BA9A-658D0F479D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516B785E-A816-714B-BC9C-14E6A0548C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="760" windowWidth="32100" windowHeight="22720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wind turbines" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="206">
   <si>
     <t>Activity</t>
   </si>
@@ -629,6 +629,36 @@
   </si>
   <si>
     <t>treatment of foundation, for offshore wind turbine</t>
+  </si>
+  <si>
+    <t>wind turbine components assembly, for wind turbine</t>
+  </si>
+  <si>
+    <t>Originally from ecoinvent v.2/3: wind power plant construction, 2MW, fixed parts [GLO]. 0.5 kWh per kilogram of component.</t>
+  </si>
+  <si>
+    <t>wind turbine installation, for onshore wind turbine</t>
+  </si>
+  <si>
+    <t>Originally from ecoinvent v.2/3: wind power plant construction, 2MW, fixed parts [GLO]. Per kilogram of onshore turbine installed.</t>
+  </si>
+  <si>
+    <t>Originally, 10 kWh of diesel burned for a 133 ton-heavy 800kW turbine.</t>
+  </si>
+  <si>
+    <t>wind turbine installation, for offshore wind turbine</t>
+  </si>
+  <si>
+    <t>Originally, 650 MJ of diesel burned for a 133 ton-heavy 800kW turbine.</t>
+  </si>
+  <si>
+    <t>Originally, 876 MJ of diesel burned for a 247 ton-heavy 2MW turbine.</t>
+  </si>
+  <si>
+    <t>excavation, hydraulic digger</t>
+  </si>
+  <si>
+    <t>market for excavation, hydraulic digger</t>
   </si>
 </sst>
 </file>
@@ -639,9 +669,16 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -710,21 +747,22 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F405F435-5E2B-E644-83D2-BBB8FE808D59}">
-  <dimension ref="A1:L464"/>
+  <dimension ref="A1:L502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A427" zoomScale="140" workbookViewId="0">
-      <selection activeCell="E445" sqref="E445"/>
+    <sheetView tabSelected="1" topLeftCell="A475" zoomScale="140" workbookViewId="0">
+      <selection activeCell="E489" sqref="E489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8436,6 +8474,487 @@
         <v>193</v>
       </c>
     </row>
+    <row r="466" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A466" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B466" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="467" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A467" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B467" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="468" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A468" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B468" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="469" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A469" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B469" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A470" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B470" s="11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="471" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A471" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B471" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="472" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A472" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B472" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="473" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A473" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="474" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A474" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B474" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C474" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D474" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E474" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F474" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G474" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H474" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I474" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J474" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K474" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L474" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A475" s="2" t="str">
+        <f>B466</f>
+        <v>wind turbine components assembly, for wind turbine</v>
+      </c>
+      <c r="B475" s="2">
+        <v>1</v>
+      </c>
+      <c r="C475" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E475" s="2" t="str">
+        <f>B468</f>
+        <v>GLO</v>
+      </c>
+      <c r="F475" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G475" s="2" t="str">
+        <f>B470</f>
+        <v>wind turbine components assembly, for wind turbine</v>
+      </c>
+    </row>
+    <row r="476" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A476" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B476" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C476" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E476" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F476" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G476" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H476"/>
+    </row>
+    <row r="478" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A478" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="479" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A479" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B479" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="480" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A480" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B480" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="481" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A481" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B481" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="482" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A482" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B482" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="483" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A483" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B483" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="484" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A484" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B484" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="485" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A485" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="486" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A486" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B486" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C486" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D486" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E486" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F486" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G486" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H486" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I486" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J486" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K486" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L486" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="487" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A487" s="2" t="str">
+        <f>B478</f>
+        <v>wind turbine installation, for onshore wind turbine</v>
+      </c>
+      <c r="B487" s="2">
+        <v>1</v>
+      </c>
+      <c r="C487" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E487" s="2" t="str">
+        <f>B480</f>
+        <v>GLO</v>
+      </c>
+      <c r="F487" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G487" s="2" t="str">
+        <f>B482</f>
+        <v>wind turbine installation, for onshore wind turbine</v>
+      </c>
+    </row>
+    <row r="488" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A488" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B488" s="2">
+        <f>(650/133000)</f>
+        <v>4.887218045112782E-3</v>
+      </c>
+      <c r="C488" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E488" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F488" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G488" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L488" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="489" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A489" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B489" s="2">
+        <f>10/133000</f>
+        <v>7.5187969924812026E-5</v>
+      </c>
+      <c r="C489" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E489" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F489" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G489" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H489"/>
+      <c r="L489" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="491" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A491" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B491" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="492" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A492" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B492" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="493" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A493" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B493" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="494" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A494" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B494" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="495" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A495" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B495" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="496" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A496" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B496" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="497" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A497" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B497" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="498" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A498" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="499" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A499" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B499" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C499" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D499" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E499" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F499" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G499" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H499" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I499" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J499" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K499" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L499" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="500" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A500" s="2" t="str">
+        <f>B491</f>
+        <v>wind turbine installation, for offshore wind turbine</v>
+      </c>
+      <c r="B500" s="2">
+        <v>1</v>
+      </c>
+      <c r="C500" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E500" s="2" t="str">
+        <f>B493</f>
+        <v>GLO</v>
+      </c>
+      <c r="F500" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G500" s="2" t="str">
+        <f>B495</f>
+        <v>wind turbine installation, for offshore wind turbine</v>
+      </c>
+    </row>
+    <row r="501" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A501" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B501" s="2">
+        <f>(876/247000)</f>
+        <v>3.5465587044534413E-3</v>
+      </c>
+      <c r="C501" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E501" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F501" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G501" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L501" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="502" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A502" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B502" s="2">
+        <f>(52500/247000)</f>
+        <v>0.2125506072874494</v>
+      </c>
+      <c r="C502" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E502" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F502" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G502" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L403" xr:uid="{F405F435-5E2B-E644-83D2-BBB8FE808D59}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>